<commit_message>
Update Graph 5 data
</commit_message>
<xml_diff>
--- a/Anna Plots/Graph 5 Ice Mass data.xlsx
+++ b/Anna Plots/Graph 5 Ice Mass data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\University UT\Year 4 Courses\STA313\Project data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\University UT\Year 4 Courses\STA313\STA313 Github\DataVisProject\Anna Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB03C683-92D1-4BCA-8398-44FC7109AD28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8E0C9D-71D5-42BF-8CB0-B46297C5840F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Average Antarctic mass 1-signma uncertainty (Gigatonnes)</t>
+    <t>Antarctic mass change (Gigatonnes)</t>
   </si>
 </sst>
 </file>
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +378,7 @@
         <v>2002</v>
       </c>
       <c r="B2">
-        <v>91.61999999999999</v>
+        <v>-6.8285714285714283</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -386,7 +386,7 @@
         <v>2003</v>
       </c>
       <c r="B3">
-        <v>44.167272727272731</v>
+        <v>-115.77363636363636</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -394,7 +394,7 @@
         <v>2004</v>
       </c>
       <c r="B4">
-        <v>37.161666666666662</v>
+        <v>-263.09500000000003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -402,7 +402,7 @@
         <v>2005</v>
       </c>
       <c r="B5">
-        <v>34.594166666666659</v>
+        <v>-229.1883333333333</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -410,7 +410,7 @@
         <v>2006</v>
       </c>
       <c r="B6">
-        <v>36.380000000000003</v>
+        <v>-130.84416666666667</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -418,7 +418,7 @@
         <v>2007</v>
       </c>
       <c r="B7">
-        <v>38.661666666666662</v>
+        <v>-317.20083333333332</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -426,7 +426,7 @@
         <v>2008</v>
       </c>
       <c r="B8">
-        <v>40.555</v>
+        <v>-587.89</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -434,7 +434,7 @@
         <v>2009</v>
       </c>
       <c r="B9">
-        <v>36.072499999999998</v>
+        <v>-563.11166666666657</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -442,7 +442,7 @@
         <v>2010</v>
       </c>
       <c r="B10">
-        <v>35.743333333333332</v>
+        <v>-841.61916666666673</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -450,7 +450,7 @@
         <v>2011</v>
       </c>
       <c r="B11">
-        <v>40.82</v>
+        <v>-940.11222222222227</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -458,7 +458,7 @@
         <v>2012</v>
       </c>
       <c r="B12">
-        <v>39.519090909090899</v>
+        <v>-1074.8372727272729</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>2013</v>
       </c>
       <c r="B13">
-        <v>38.198888888888888</v>
+        <v>-1285.1311111111111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -474,7 +474,7 @@
         <v>2014</v>
       </c>
       <c r="B14">
-        <v>33.766666666666666</v>
+        <v>-1495.9399999999998</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -482,7 +482,7 @@
         <v>2015</v>
       </c>
       <c r="B15">
-        <v>37.300000000000004</v>
+        <v>-1847.6000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -490,7 +490,7 @@
         <v>2016</v>
       </c>
       <c r="B16">
-        <v>41.071111111111115</v>
+        <v>-1769.5422222222221</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -498,7 +498,7 @@
         <v>2017</v>
       </c>
       <c r="B17">
-        <v>60.703999999999994</v>
+        <v>-1803.23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>2018</v>
       </c>
       <c r="B18">
-        <v>30.488</v>
+        <v>-2147.9679999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -514,7 +514,7 @@
         <v>2019</v>
       </c>
       <c r="B19">
-        <v>26.855</v>
+        <v>-2269.3016666666667</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -522,7 +522,15 @@
         <v>2020</v>
       </c>
       <c r="B20">
-        <v>31.902500000000003</v>
+        <v>-2542.3516666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21">
+        <v>-2913.3050000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>